<commit_message>
standardizing text data, removing text from numerical data
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yotam\Documents\Grant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F272A21E-F102-441E-9482-CA0CF5CB60B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A51F91-41EE-4A60-AA81-3C59C1E868ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>2 hours</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>people</t>
+  </si>
+  <si>
+    <t>1.25 hours</t>
   </si>
 </sst>
 </file>
@@ -393,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,6 +480,20 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>45674</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Convert .csv to .xlsx, sign form, adjust hours
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yotam\Documents\Grant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A51F91-41EE-4A60-AA81-3C59C1E868ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB85CDEC-CD86-4479-BFF5-31B564BC7EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>2 hours</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>1.25 hours</t>
+  </si>
+  <si>
+    <t>cleaning and sharing data, reviewing email text</t>
+  </si>
+  <si>
+    <t>.5 hours</t>
   </si>
 </sst>
 </file>
@@ -396,17 +402,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -494,6 +500,20 @@
         <v>8</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>45679</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Clean properties data, update hours
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yotam\Documents\Grant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB375B5-B0CB-4693-A7D7-A8BA656ACBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725D01FC-5040-465C-A7BA-346BD7C40631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="324" yWindow="0" windowWidth="16836" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>2 hours</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>1 hour</t>
+  </si>
+  <si>
+    <t>clean properties data</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,6 +545,17 @@
         <v>16</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>45695</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update plots and hours
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yotam\Documents\Grant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725D01FC-5040-465C-A7BA-346BD7C40631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78435248-E5D1-4616-8AE5-D3A5AF557AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>2 hours</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>clean properties data</t>
+  </si>
+  <si>
+    <t>1 hours</t>
+  </si>
+  <si>
+    <t>discuss plots and next steps</t>
   </si>
 </sst>
 </file>
@@ -411,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,6 +562,20 @@
         <v>18</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>45725</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
generate plot and adjust hours
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yotam\Documents\Grant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF44DD6-6144-41FA-A4EB-D82FED9FF5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680D26C9-4DF5-4209-A93C-AB9E449882E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,7 +584,7 @@
         <v>45729</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
print plots and add titles
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yotam\Documents\Grant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9BBDDB-5AAC-4E91-A2F8-826A4EE02CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB389D0-CB17-4C1A-87C7-FEA8FB08669E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>2 hours</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>plotting new data</t>
+  </si>
+  <si>
+    <t>printing plots and adding titles</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,6 +644,17 @@
         <v>26</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>45736</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update data and plots
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yotam\Documents\Grant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB389D0-CB17-4C1A-87C7-FEA8FB08669E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7D8F10-281F-4731-9154-420BA26C1A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6312" yWindow="1332" windowWidth="14640" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>2 hours</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>printing plots and adding titles</t>
+  </si>
+  <si>
+    <t>Update data and plots</t>
   </si>
 </sst>
 </file>
@@ -438,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,6 +658,17 @@
         <v>27</v>
       </c>
     </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>45737</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
write and edit report
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yotam\Documents\Grant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7D8F10-281F-4731-9154-420BA26C1A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C529A8-0BE3-4EFE-BB3C-9B804170ABB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6312" yWindow="1332" windowWidth="14640" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>2 hours</t>
   </si>
@@ -122,7 +122,10 @@
     <t>printing plots and adding titles</t>
   </si>
   <si>
-    <t>Update data and plots</t>
+    <t>update data and plots</t>
+  </si>
+  <si>
+    <t>write and edit report</t>
   </si>
 </sst>
 </file>
@@ -441,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B2" sqref="B2:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,6 +672,17 @@
         <v>28</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>45737</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>